<commit_message>
Insertando al proyecto el diseño de la base de datos del hospedaje
</commit_message>
<xml_diff>
--- a/Analisis De Registro De Huesped.xlsx
+++ b/Analisis De Registro De Huesped.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Hostal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548D0EFC-44D1-4DCD-A8EC-FC79AAE70C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF14E240-B6D0-4E6A-8ECE-FF1498882CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{27382F85-EFBF-4DEB-9D13-3D1A750AE910}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="188">
   <si>
     <t>id</t>
   </si>
@@ -575,6 +575,30 @@
   </si>
   <si>
     <t>DESCRIPCIÓN</t>
+  </si>
+  <si>
+    <t>RESERVAR</t>
+  </si>
+  <si>
+    <t>Fecha_Estamcia</t>
+  </si>
+  <si>
+    <t>Fecha_Salda</t>
+  </si>
+  <si>
+    <t>RESERVAR - HABITACIONES</t>
+  </si>
+  <si>
+    <t>HABITACION.ID</t>
+  </si>
+  <si>
+    <t>RESERVAR.ID</t>
+  </si>
+  <si>
+    <t>Fecha_Atención</t>
+  </si>
+  <si>
+    <t>Numero Personas</t>
   </si>
 </sst>
 </file>
@@ -993,14 +1017,13 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1190,9 +1213,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1202,24 +1246,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1229,11 +1255,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="12" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2269,15 +2305,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>793377</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76198</xdr:rowOff>
+      <xdr:colOff>771605</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>87084</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>316006</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>94129</xdr:rowOff>
+      <xdr:colOff>294234</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>105015</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2292,8 +2328,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23443827" y="2362198"/>
-          <a:ext cx="4323229" cy="5999631"/>
+          <a:off x="25536605" y="2862941"/>
+          <a:ext cx="5335600" cy="5885331"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2947,10 +2983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3055721-4A3A-49D5-A5B0-B5D229A0D2E2}">
-  <dimension ref="B2:R58"/>
+  <dimension ref="B2:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2966,31 +3002,37 @@
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
     <col min="11" max="12" width="27" customWidth="1"/>
     <col min="13" max="13" width="22.21875" customWidth="1"/>
-    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" customWidth="1"/>
     <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="24.21875" customWidth="1"/>
+    <col min="17" max="17" width="25.109375" customWidth="1"/>
+    <col min="18" max="18" width="23.6640625" customWidth="1"/>
+    <col min="19" max="19" width="24.88671875" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C2" s="90" t="s">
+    <row r="2" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C2" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90" t="s">
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="K2" s="90" t="s">
+      <c r="H2" s="95"/>
+      <c r="K2" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-    </row>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+    </row>
+    <row r="3" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3000,7 +3042,7 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="103" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -3028,7 +3070,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C4" s="1">
         <v>11111111</v>
       </c>
@@ -3038,7 +3080,7 @@
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="104">
         <v>36524</v>
       </c>
       <c r="G4" s="1">
@@ -3066,7 +3108,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C5" s="1">
         <v>22222222</v>
       </c>
@@ -3076,7 +3118,7 @@
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="104">
         <v>34175</v>
       </c>
       <c r="G5" s="1">
@@ -3104,7 +3146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C6" s="1">
         <v>33333333</v>
       </c>
@@ -3114,7 +3156,7 @@
       <c r="E6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="104">
         <v>34380</v>
       </c>
       <c r="G6" s="1">
@@ -3124,7 +3166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>44444444</v>
       </c>
@@ -3134,7 +3176,7 @@
       <c r="E7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="104">
         <v>19946</v>
       </c>
       <c r="G7" s="1">
@@ -3144,7 +3186,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>55555555</v>
       </c>
@@ -3154,7 +3196,7 @@
       <c r="E8" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="104">
         <v>16659</v>
       </c>
       <c r="G8" s="3">
@@ -3163,14 +3205,20 @@
       <c r="H8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K8" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="11"/>
+      <c r="S8" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>66666666</v>
       </c>
@@ -3180,7 +3228,7 @@
       <c r="E9" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="104">
         <v>25049</v>
       </c>
       <c r="G9" s="3">
@@ -3189,42 +3237,123 @@
       <c r="H9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="R9" s="11"/>
+      <c r="S9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C12" s="90" t="s">
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>7</v>
+      </c>
+      <c r="N10" s="1">
+        <v>3</v>
+      </c>
+      <c r="O10" s="2">
+        <v>44064</v>
+      </c>
+      <c r="P10" s="105">
+        <v>44037</v>
+      </c>
+      <c r="Q10" s="105">
+        <v>44042</v>
+      </c>
+      <c r="R10" s="11"/>
+      <c r="S10" s="1">
+        <v>1</v>
+      </c>
+      <c r="T10" s="3">
+        <v>1</v>
+      </c>
+      <c r="U10" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="K11" s="1">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="S11" s="1">
+        <v>2</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C12" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="91" t="s">
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="92"/>
-      <c r="I12" s="93"/>
-      <c r="R12" s="6"/>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="H12" s="98"/>
+      <c r="I12" s="99"/>
+      <c r="K12" s="1">
+        <v>3</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="106"/>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
@@ -3246,9 +3375,20 @@
       <c r="I13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R13" s="7"/>
-    </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <v>4</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="3"/>
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <v>76039986</v>
       </c>
@@ -3270,9 +3410,9 @@
       <c r="I14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R14" s="8"/>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
         <v>76039987</v>
       </c>
@@ -3294,55 +3434,55 @@
       <c r="I15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R15" s="8"/>
-    </row>
-    <row r="16" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="R15" s="7"/>
+    </row>
+    <row r="16" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="60"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="59"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="61"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="15" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="95" t="s">
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="L18" s="95"/>
-      <c r="M18" s="17" t="s">
+      <c r="L18" s="96"/>
+      <c r="M18" s="16" t="s">
         <v>60</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O18" s="11"/>
-      <c r="P18" s="62"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="61"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="61"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
@@ -3367,10 +3507,10 @@
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K19" s="90" t="s">
+      <c r="K19" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="L19" s="90"/>
+      <c r="L19" s="95"/>
       <c r="M19" s="1" t="s">
         <v>41</v>
       </c>
@@ -3380,10 +3520,10 @@
       <c r="O19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="P19" s="62"/>
+      <c r="P19" s="61"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="61"/>
+      <c r="B20" s="60"/>
       <c r="C20" s="1">
         <v>1</v>
       </c>
@@ -3393,7 +3533,7 @@
       <c r="E20" s="1">
         <v>1</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>67</v>
       </c>
       <c r="G20" s="1">
@@ -3405,26 +3545,26 @@
       <c r="I20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="K20" s="90">
+      <c r="K20" s="95">
         <v>1</v>
       </c>
-      <c r="L20" s="90"/>
-      <c r="M20" s="28">
+      <c r="L20" s="95"/>
+      <c r="M20" s="27">
         <v>1</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="O20" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="P20" s="62"/>
+      <c r="P20" s="61"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B21" s="61"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="1">
         <v>2</v>
       </c>
@@ -3434,7 +3574,7 @@
       <c r="E21" s="1">
         <v>2</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="8" t="s">
         <v>67</v>
       </c>
       <c r="G21" s="1">
@@ -3449,23 +3589,23 @@
       <c r="J21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K21" s="90">
+      <c r="K21" s="95">
         <v>2</v>
       </c>
-      <c r="L21" s="90"/>
-      <c r="M21" s="28">
+      <c r="L21" s="95"/>
+      <c r="M21" s="27">
         <v>2</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O21" s="9" t="s">
+      <c r="O21" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="P21" s="62"/>
+      <c r="P21" s="61"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="61"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="1">
         <v>3</v>
       </c>
@@ -3475,7 +3615,7 @@
       <c r="E22" s="1">
         <v>3</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>67</v>
       </c>
       <c r="G22" s="1">
@@ -3490,23 +3630,23 @@
       <c r="J22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K22" s="96">
+      <c r="K22" s="91">
         <v>1</v>
       </c>
-      <c r="L22" s="97"/>
-      <c r="M22" s="28">
+      <c r="L22" s="92"/>
+      <c r="M22" s="27">
         <v>1</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O22" s="34" t="s">
+      <c r="O22" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="P22" s="62"/>
+      <c r="P22" s="61"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23" s="61"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="1">
         <v>4</v>
       </c>
@@ -3516,7 +3656,7 @@
       <c r="E23" s="1">
         <v>4</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="8" t="s">
         <v>67</v>
       </c>
       <c r="G23" s="1">
@@ -3531,62 +3671,62 @@
       <c r="J23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K23" s="99">
+      <c r="K23" s="94">
         <v>4</v>
       </c>
-      <c r="L23" s="99"/>
-      <c r="M23" s="28">
+      <c r="L23" s="94"/>
+      <c r="M23" s="27">
         <v>4</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O23" s="34" t="s">
+      <c r="O23" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="P23" s="62"/>
-    </row>
-    <row r="24" spans="2:16" s="70" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="71"/>
-      <c r="C24" s="23">
+      <c r="P23" s="61"/>
+    </row>
+    <row r="24" spans="2:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="70"/>
+      <c r="C24" s="22">
         <v>5</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="22">
         <v>202</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="22">
         <v>5</v>
       </c>
-      <c r="F24" s="72" t="s">
+      <c r="F24" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="22">
         <v>1</v>
       </c>
-      <c r="H24" s="73">
+      <c r="H24" s="72">
         <v>43764</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="K24" s="98">
+      <c r="K24" s="93">
         <v>3</v>
       </c>
-      <c r="L24" s="98"/>
-      <c r="M24" s="74">
+      <c r="L24" s="93"/>
+      <c r="M24" s="73">
         <v>1</v>
       </c>
-      <c r="N24" s="23" t="s">
+      <c r="N24" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="O24" s="23"/>
-      <c r="P24" s="75"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="74"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B25" s="61"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="1">
         <v>6</v>
       </c>
@@ -3596,7 +3736,7 @@
       <c r="E25" s="1">
         <v>6</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="8" t="s">
         <v>67</v>
       </c>
       <c r="G25" s="1">
@@ -3611,99 +3751,99 @@
       <c r="J25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K25" s="99">
+      <c r="K25" s="94">
         <v>2</v>
       </c>
-      <c r="L25" s="99"/>
-      <c r="M25" s="28">
+      <c r="L25" s="94"/>
+      <c r="M25" s="27">
         <v>2</v>
       </c>
-      <c r="N25" s="23" t="s">
+      <c r="N25" s="22" t="s">
         <v>45</v>
       </c>
       <c r="O25" s="1"/>
-      <c r="P25" s="62"/>
+      <c r="P25" s="61"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="61"/>
+      <c r="B26" s="60"/>
       <c r="C26" s="1">
         <v>6</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="9"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="1"/>
       <c r="H26" s="2"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="99"/>
-      <c r="L26" s="99"/>
-      <c r="M26" s="28"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="94"/>
+      <c r="M26" s="27"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="62"/>
+      <c r="P26" s="61"/>
     </row>
     <row r="27" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="63"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="65"/>
-    </row>
-    <row r="29" spans="2:16" s="31" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="14" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="64"/>
+    </row>
+    <row r="29" spans="2:16" s="30" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="H29" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="K29" s="32" t="s">
+      <c r="K29" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="L29" s="32" t="s">
+      <c r="L29" s="31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="2:16" s="31" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="14" t="s">
+    <row r="30" spans="2:16" s="30" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="94" t="s">
+      <c r="D30" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="94"/>
-      <c r="F30" s="19" t="s">
+      <c r="E30" s="107"/>
+      <c r="F30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="18" t="s">
+      <c r="I30" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="J30" s="18" t="s">
+      <c r="J30" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="K30" s="19" t="s">
+      <c r="K30" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L30" s="19" t="s">
+      <c r="L30" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="M30" s="19" t="s">
+      <c r="M30" s="18" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3711,11 +3851,11 @@
       <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" s="90">
+      <c r="D31" s="108">
         <v>1</v>
       </c>
-      <c r="E31" s="90"/>
-      <c r="F31" s="25">
+      <c r="E31" s="108"/>
+      <c r="F31" s="24">
         <v>2</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -3724,16 +3864,16 @@
       <c r="H31" s="2">
         <v>43758</v>
       </c>
-      <c r="I31" s="16">
+      <c r="I31" s="15">
         <v>202</v>
       </c>
-      <c r="J31" s="16">
+      <c r="J31" s="15">
         <v>30</v>
       </c>
       <c r="K31" s="1">
         <v>0</v>
       </c>
-      <c r="L31" s="9" t="s">
+      <c r="L31" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M31" s="5">
@@ -3745,11 +3885,11 @@
       <c r="C32" s="1">
         <v>2</v>
       </c>
-      <c r="D32" s="90">
+      <c r="D32" s="108">
         <v>2</v>
       </c>
-      <c r="E32" s="90"/>
-      <c r="F32" s="25">
+      <c r="E32" s="108"/>
+      <c r="F32" s="24">
         <v>2</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -3758,16 +3898,16 @@
       <c r="H32" s="2">
         <v>43759</v>
       </c>
-      <c r="I32" s="16">
+      <c r="I32" s="15">
         <v>201</v>
       </c>
-      <c r="J32" s="16">
+      <c r="J32" s="15">
         <v>30</v>
       </c>
-      <c r="K32" s="24">
+      <c r="K32" s="23">
         <v>20</v>
       </c>
-      <c r="L32" s="9" t="s">
+      <c r="L32" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M32" s="5">
@@ -3779,11 +3919,11 @@
       <c r="C33" s="1">
         <v>3</v>
       </c>
-      <c r="D33" s="90">
+      <c r="D33" s="108">
         <v>2</v>
       </c>
-      <c r="E33" s="90"/>
-      <c r="F33" s="25">
+      <c r="E33" s="108"/>
+      <c r="F33" s="24">
         <v>2</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -3792,16 +3932,16 @@
       <c r="H33" s="2">
         <v>43760</v>
       </c>
-      <c r="I33" s="16">
+      <c r="I33" s="15">
         <v>201</v>
       </c>
-      <c r="J33" s="16">
+      <c r="J33" s="15">
         <v>30</v>
       </c>
       <c r="K33" s="1">
         <v>0</v>
       </c>
-      <c r="L33" s="14" t="s">
+      <c r="L33" s="13" t="s">
         <v>64</v>
       </c>
       <c r="M33" s="5">
@@ -3813,11 +3953,11 @@
       <c r="C34" s="1">
         <v>4</v>
       </c>
-      <c r="D34" s="90">
+      <c r="D34" s="108">
         <v>3</v>
       </c>
-      <c r="E34" s="90"/>
-      <c r="F34" s="25">
+      <c r="E34" s="108"/>
+      <c r="F34" s="24">
         <v>2</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -3826,16 +3966,16 @@
       <c r="H34" s="2">
         <v>43759</v>
       </c>
-      <c r="I34" s="16">
+      <c r="I34" s="15">
         <v>202</v>
       </c>
-      <c r="J34" s="16">
+      <c r="J34" s="15">
         <v>30</v>
       </c>
       <c r="K34" s="1">
         <v>0</v>
       </c>
-      <c r="L34" s="9" t="s">
+      <c r="L34" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M34" s="5">
@@ -3847,11 +3987,11 @@
       <c r="C35" s="1">
         <v>5</v>
       </c>
-      <c r="D35" s="96">
+      <c r="D35" s="109">
         <v>4</v>
       </c>
-      <c r="E35" s="97"/>
-      <c r="F35" s="25">
+      <c r="E35" s="110"/>
+      <c r="F35" s="24">
         <v>2</v>
       </c>
       <c r="G35" s="1" t="s">
@@ -3860,16 +4000,16 @@
       <c r="H35" s="2">
         <v>43760</v>
       </c>
-      <c r="I35" s="16">
+      <c r="I35" s="15">
         <v>202</v>
       </c>
-      <c r="J35" s="16">
+      <c r="J35" s="15">
         <v>30</v>
       </c>
       <c r="K35" s="1">
         <v>0</v>
       </c>
-      <c r="L35" s="9" t="s">
+      <c r="L35" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M35" s="5">
@@ -3881,11 +4021,11 @@
       <c r="C36" s="1">
         <v>6</v>
       </c>
-      <c r="D36" s="96">
+      <c r="D36" s="109">
         <v>4</v>
       </c>
-      <c r="E36" s="97"/>
-      <c r="F36" s="25">
+      <c r="E36" s="110"/>
+      <c r="F36" s="24">
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
@@ -3894,16 +4034,16 @@
       <c r="H36" s="2">
         <v>43761</v>
       </c>
-      <c r="I36" s="16">
+      <c r="I36" s="15">
         <v>202</v>
       </c>
-      <c r="J36" s="16">
+      <c r="J36" s="15">
         <v>30</v>
       </c>
       <c r="K36" s="1">
         <v>0</v>
       </c>
-      <c r="L36" s="9" t="s">
+      <c r="L36" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M36" s="5">
@@ -3915,11 +4055,11 @@
       <c r="C37" s="1">
         <v>7</v>
       </c>
-      <c r="D37" s="96">
+      <c r="D37" s="109">
         <v>4</v>
       </c>
-      <c r="E37" s="97"/>
-      <c r="F37" s="25">
+      <c r="E37" s="110"/>
+      <c r="F37" s="24">
         <v>2</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -3928,16 +4068,16 @@
       <c r="H37" s="2">
         <v>43762</v>
       </c>
-      <c r="I37" s="16">
+      <c r="I37" s="15">
         <v>202</v>
       </c>
-      <c r="J37" s="16">
+      <c r="J37" s="15">
         <v>30</v>
       </c>
       <c r="K37" s="1">
         <v>0</v>
       </c>
-      <c r="L37" s="9" t="s">
+      <c r="L37" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M37" s="5">
@@ -3949,11 +4089,11 @@
       <c r="C38" s="1">
         <v>8</v>
       </c>
-      <c r="D38" s="96">
+      <c r="D38" s="109">
         <v>4</v>
       </c>
-      <c r="E38" s="97"/>
-      <c r="F38" s="25">
+      <c r="E38" s="110"/>
+      <c r="F38" s="24">
         <v>2</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -3962,16 +4102,16 @@
       <c r="H38" s="2">
         <v>43763</v>
       </c>
-      <c r="I38" s="16">
+      <c r="I38" s="15">
         <v>202</v>
       </c>
-      <c r="J38" s="16">
+      <c r="J38" s="15">
         <v>30</v>
       </c>
       <c r="K38" s="1">
         <v>0</v>
       </c>
-      <c r="L38" s="9" t="s">
+      <c r="L38" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M38" s="5">
@@ -3986,29 +4126,29 @@
       <c r="C39" s="1">
         <v>9</v>
       </c>
-      <c r="D39" s="96">
+      <c r="D39" s="109">
         <v>5</v>
       </c>
-      <c r="E39" s="97"/>
-      <c r="F39" s="25">
+      <c r="E39" s="110"/>
+      <c r="F39" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="23" t="s">
+      <c r="G39" s="22" t="s">
         <v>111</v>
       </c>
       <c r="H39" s="2">
         <v>43764</v>
       </c>
-      <c r="I39" s="16">
+      <c r="I39" s="15">
         <v>202</v>
       </c>
-      <c r="J39" s="16">
+      <c r="J39" s="15">
         <v>30</v>
       </c>
       <c r="K39" s="1">
         <v>0</v>
       </c>
-      <c r="L39" s="9" t="s">
+      <c r="L39" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M39" s="5">
@@ -4020,11 +4160,11 @@
       <c r="C40" s="1">
         <v>10</v>
       </c>
-      <c r="D40" s="96">
+      <c r="D40" s="109">
         <v>6</v>
       </c>
-      <c r="E40" s="97"/>
-      <c r="F40" s="25">
+      <c r="E40" s="110"/>
+      <c r="F40" s="24">
         <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
@@ -4033,16 +4173,16 @@
       <c r="H40" s="2">
         <v>43764</v>
       </c>
-      <c r="I40" s="16">
+      <c r="I40" s="15">
         <v>201</v>
       </c>
-      <c r="J40" s="16">
+      <c r="J40" s="15">
         <v>30</v>
       </c>
       <c r="K40" s="1">
         <v>0</v>
       </c>
-      <c r="L40" s="9" t="s">
+      <c r="L40" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M40" s="5">
@@ -4054,11 +4194,11 @@
       <c r="C41" s="1">
         <v>11</v>
       </c>
-      <c r="D41" s="96">
+      <c r="D41" s="109">
         <v>6</v>
       </c>
-      <c r="E41" s="97"/>
-      <c r="F41" s="25">
+      <c r="E41" s="110"/>
+      <c r="F41" s="24">
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
@@ -4067,16 +4207,16 @@
       <c r="H41" s="2">
         <v>43765</v>
       </c>
-      <c r="I41" s="16">
+      <c r="I41" s="15">
         <v>201</v>
       </c>
-      <c r="J41" s="16">
+      <c r="J41" s="15">
         <v>30</v>
       </c>
       <c r="K41" s="1">
         <v>0</v>
       </c>
-      <c r="L41" s="9" t="s">
+      <c r="L41" s="8" t="s">
         <v>66</v>
       </c>
       <c r="M41" s="5">
@@ -4088,30 +4228,30 @@
       <c r="C42" s="1">
         <v>12</v>
       </c>
-      <c r="D42" s="96"/>
-      <c r="E42" s="97"/>
-      <c r="F42" s="25"/>
+      <c r="D42" s="109"/>
+      <c r="E42" s="110"/>
+      <c r="F42" s="24"/>
       <c r="G42" s="1"/>
       <c r="H42" s="2"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="9"/>
+      <c r="L42" s="8"/>
       <c r="M42" s="5"/>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C43" s="1">
         <v>13</v>
       </c>
-      <c r="D43" s="96"/>
-      <c r="E43" s="97"/>
-      <c r="F43" s="25"/>
+      <c r="D43" s="109"/>
+      <c r="E43" s="110"/>
+      <c r="F43" s="24"/>
       <c r="G43" s="1"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="9"/>
+      <c r="L43" s="8"/>
       <c r="M43" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4128,10 +4268,10 @@
       </c>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -4145,10 +4285,10 @@
       </c>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C48" s="20">
+      <c r="C48" s="19">
         <v>1</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="20">
         <v>43671</v>
       </c>
       <c r="E48" s="4">
@@ -4162,10 +4302,10 @@
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C49" s="20">
+      <c r="C49" s="19">
         <v>2</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="20">
         <v>43466</v>
       </c>
       <c r="E49" s="4">
@@ -4179,10 +4319,10 @@
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C50" s="20">
+      <c r="C50" s="19">
         <v>3</v>
       </c>
-      <c r="D50" s="21">
+      <c r="D50" s="20">
         <v>43760</v>
       </c>
       <c r="E50" s="4">
@@ -4201,7 +4341,7 @@
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C54" s="23" t="s">
+      <c r="C54" s="22" t="s">
         <v>0</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -4218,16 +4358,16 @@
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C55" s="23">
+      <c r="C55" s="22">
         <v>1</v>
       </c>
-      <c r="D55" s="21">
+      <c r="D55" s="20">
         <v>43671</v>
       </c>
       <c r="E55" s="1">
         <v>201</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="9">
         <v>0</v>
       </c>
       <c r="G55" s="1">
@@ -4235,16 +4375,16 @@
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C56" s="23">
+      <c r="C56" s="22">
         <v>2</v>
       </c>
-      <c r="D56" s="21">
+      <c r="D56" s="20">
         <v>43671</v>
       </c>
       <c r="E56" s="1">
         <v>202</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="9">
         <v>0</v>
       </c>
       <c r="G56" s="1">
@@ -4252,33 +4392,33 @@
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C57" s="23">
+      <c r="C57" s="22">
         <v>3</v>
       </c>
-      <c r="D57" s="21">
+      <c r="D57" s="20">
         <v>43760</v>
       </c>
       <c r="E57" s="1">
         <v>201</v>
       </c>
-      <c r="F57" s="10">
+      <c r="F57" s="9">
         <v>0</v>
       </c>
-      <c r="G57" s="24">
+      <c r="G57" s="23">
         <v>20</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C58" s="23">
+      <c r="C58" s="22">
         <v>4</v>
       </c>
-      <c r="D58" s="21">
+      <c r="D58" s="20">
         <v>43760</v>
       </c>
       <c r="E58" s="1">
         <v>202</v>
       </c>
-      <c r="F58" s="10">
+      <c r="F58" s="9">
         <v>0</v>
       </c>
       <c r="G58" s="1">
@@ -4287,6 +4427,25 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="K25:L25"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
@@ -4296,25 +4455,6 @@
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="D41:E41"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D33:E33"/>
   </mergeCells>
   <conditionalFormatting sqref="N20:N25">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="BUENO">
@@ -4343,10 +4483,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="31" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" style="89" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" style="89" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="31" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="30" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" style="88" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="88" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4358,338 +4498,338 @@
       <c r="E2" s="102"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="82" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="51"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="50"/>
       <c r="F3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="103"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="89"/>
       <c r="F4" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="103"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="89"/>
       <c r="F5" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="83" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="103"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="89"/>
       <c r="F6" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="103"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="89"/>
       <c r="F7" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="80" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="84" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="53"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="52"/>
       <c r="F8" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="104" t="s">
+      <c r="C12" s="90" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="90" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="82" t="s">
+      <c r="E12" s="81" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="81" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="90" t="s">
         <v>153</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="E13" s="82" t="s">
+      <c r="E13" s="81" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="81" t="s">
         <v>137</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="81" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="90" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="104" t="s">
+      <c r="D15" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="E15" s="82" t="s">
+      <c r="E15" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="90" t="s">
         <v>156</v>
       </c>
-      <c r="D16" s="104" t="s">
+      <c r="D16" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="82" t="s">
+      <c r="E16" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="81" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="D17" s="104" t="s">
+      <c r="D17" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="82" t="s">
+      <c r="E17" s="81" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="90" t="s">
         <v>158</v>
       </c>
-      <c r="D18" s="104" t="s">
+      <c r="D18" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="82" t="s">
+      <c r="E18" s="81" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="104" t="s">
+      <c r="C19" s="90" t="s">
         <v>159</v>
       </c>
-      <c r="D19" s="104" t="s">
+      <c r="D19" s="90" t="s">
         <v>176</v>
       </c>
-      <c r="E19" s="82" t="s">
+      <c r="E19" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="81" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="104" t="s">
+      <c r="C20" s="90" t="s">
         <v>160</v>
       </c>
-      <c r="D20" s="104" t="s">
+      <c r="D20" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="81" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="104" t="s">
+      <c r="C21" s="90" t="s">
         <v>161</v>
       </c>
-      <c r="D21" s="104" t="s">
+      <c r="D21" s="90" t="s">
         <v>172</v>
       </c>
-      <c r="E21" s="82" t="s">
+      <c r="E21" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="C22" s="104" t="s">
+      <c r="C22" s="90" t="s">
         <v>162</v>
       </c>
-      <c r="D22" s="104" t="s">
+      <c r="D22" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="82" t="s">
+      <c r="E22" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="C23" s="104" t="s">
+      <c r="C23" s="90" t="s">
         <v>163</v>
       </c>
-      <c r="D23" s="104" t="s">
+      <c r="D23" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="82" t="s">
+      <c r="E23" s="81" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="104" t="s">
+      <c r="C24" s="90" t="s">
         <v>164</v>
       </c>
-      <c r="D24" s="104" t="s">
+      <c r="D24" s="90" t="s">
         <v>172</v>
       </c>
-      <c r="E24" s="82" t="s">
+      <c r="E24" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="C25" s="104" t="s">
+      <c r="C25" s="90" t="s">
         <v>165</v>
       </c>
-      <c r="D25" s="104" t="s">
+      <c r="D25" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="82" t="s">
+      <c r="E25" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="104" t="s">
+      <c r="C26" s="90" t="s">
         <v>166</v>
       </c>
-      <c r="D26" s="104" t="s">
+      <c r="D26" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="82" t="s">
+      <c r="E26" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="82" t="s">
+      <c r="B27" s="81" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="104" t="s">
+      <c r="C27" s="90" t="s">
         <v>167</v>
       </c>
-      <c r="D27" s="104" t="s">
+      <c r="D27" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="E27" s="82" t="s">
+      <c r="E27" s="81" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="82" t="s">
+      <c r="B28" s="81" t="s">
         <v>151</v>
       </c>
-      <c r="C28" s="104" t="s">
+      <c r="C28" s="90" t="s">
         <v>168</v>
       </c>
-      <c r="D28" s="104" t="s">
+      <c r="D28" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="E28" s="82" t="s">
+      <c r="E28" s="81" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="82" t="s">
+      <c r="B29" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="C29" s="104" t="s">
+      <c r="C29" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="D29" s="104" t="s">
+      <c r="D29" s="90" t="s">
         <v>173</v>
       </c>
-      <c r="E29" s="82" t="s">
+      <c r="E29" s="81" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4728,24 +4868,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="J2" s="90" t="s">
+      <c r="G2" s="95"/>
+      <c r="J2" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -4882,17 +5022,17 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="90" t="s">
+      <c r="B9" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91" t="s">
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="92"/>
-      <c r="H9" s="93"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="99"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -4964,17 +5104,17 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91" t="s">
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="92"/>
-      <c r="H15" s="93"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="99"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
@@ -5024,7 +5164,7 @@
       <c r="H17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="K17" s="25" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5050,405 +5190,405 @@
       <c r="H18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="27" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K19" s="34" t="s">
+      <c r="K19" s="33" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="79" t="s">
+      <c r="F21" s="78" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="55" t="s">
+      <c r="D22" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="55" t="s">
+      <c r="E22" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="56" t="s">
+      <c r="G22" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="54" t="s">
+      <c r="H22" s="53" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="23" spans="2:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="37"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="67" t="s">
+      <c r="B23" s="36"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="H23" s="54"/>
+      <c r="H23" s="53"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="51">
+      <c r="B24" s="50">
         <v>1</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="40">
         <v>1</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="44">
         <v>202</v>
       </c>
-      <c r="E24" s="46">
+      <c r="E24" s="45">
         <v>43758</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="43">
         <v>43759</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H24" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="27">
+      <c r="B25" s="26">
         <v>2</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="25">
         <v>2</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="46">
         <v>201</v>
       </c>
-      <c r="E25" s="48">
+      <c r="E25" s="47">
         <v>43759</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="42">
         <v>43760</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="37">
+      <c r="B26" s="36">
         <v>4</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="25">
         <v>2</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="48">
         <v>201</v>
       </c>
-      <c r="E26" s="50">
+      <c r="E26" s="49">
         <v>43760</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="42">
         <v>43761</v>
       </c>
-      <c r="G26" s="52" t="s">
+      <c r="G26" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="38">
+      <c r="B27" s="37">
         <v>3</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="25">
         <v>3</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="46">
         <v>202</v>
       </c>
-      <c r="E27" s="48">
+      <c r="E27" s="47">
         <v>43759</v>
       </c>
-      <c r="F27" s="43">
+      <c r="F27" s="42">
         <v>43760</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="H27" s="35" t="s">
+      <c r="H27" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="27">
+      <c r="B28" s="26">
         <v>5</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="25">
         <v>4</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D28" s="46">
         <v>202</v>
       </c>
-      <c r="E28" s="48">
+      <c r="E28" s="47">
         <v>43760</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="42">
         <v>43761</v>
       </c>
-      <c r="G28" s="52" t="s">
+      <c r="G28" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="30">
+      <c r="B29" s="29">
         <v>6</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="25">
         <v>4</v>
       </c>
-      <c r="D29" s="68">
+      <c r="D29" s="67">
         <v>202</v>
       </c>
-      <c r="E29" s="69">
+      <c r="E29" s="68">
         <v>43761</v>
       </c>
-      <c r="F29" s="43">
+      <c r="F29" s="42">
         <v>43762</v>
       </c>
-      <c r="G29" s="67" t="s">
+      <c r="G29" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="H29" s="35" t="s">
+      <c r="H29" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="27">
+      <c r="B30" s="26">
         <v>7</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="25">
         <v>4</v>
       </c>
-      <c r="D30" s="68">
+      <c r="D30" s="67">
         <v>202</v>
       </c>
-      <c r="E30" s="69">
+      <c r="E30" s="68">
         <v>43762</v>
       </c>
-      <c r="F30" s="43">
+      <c r="F30" s="42">
         <v>43763</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H30" s="35" t="s">
+      <c r="H30" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="30">
+      <c r="B31" s="29">
         <v>8</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="25">
         <v>4</v>
       </c>
-      <c r="D31" s="49">
+      <c r="D31" s="48">
         <v>202</v>
       </c>
-      <c r="E31" s="50">
+      <c r="E31" s="49">
         <v>43763</v>
       </c>
-      <c r="F31" s="43">
+      <c r="F31" s="42">
         <v>43764</v>
       </c>
-      <c r="G31" s="67" t="s">
+      <c r="G31" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="H31" s="35" t="s">
+      <c r="H31" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="27">
+      <c r="B32" s="26">
         <v>9</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="25">
         <v>5</v>
       </c>
-      <c r="D32" s="47">
+      <c r="D32" s="46">
         <v>202</v>
       </c>
-      <c r="E32" s="48">
+      <c r="E32" s="47">
         <v>43764</v>
       </c>
-      <c r="F32" s="43">
+      <c r="F32" s="42">
         <v>43765</v>
       </c>
-      <c r="G32" s="29" t="s">
+      <c r="G32" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="57">
+      <c r="B33" s="56">
         <v>11</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="41">
         <v>5</v>
       </c>
-      <c r="D33" s="77">
+      <c r="D33" s="76">
         <v>202</v>
       </c>
-      <c r="E33" s="69">
+      <c r="E33" s="68">
         <v>43765</v>
       </c>
-      <c r="F33" s="44">
+      <c r="F33" s="43">
         <v>43766</v>
       </c>
-      <c r="G33" s="66" t="s">
+      <c r="G33" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="35" t="s">
+      <c r="H33" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="37">
+      <c r="B34" s="36">
         <v>13</v>
       </c>
-      <c r="C34" s="35">
+      <c r="C34" s="34">
         <v>5</v>
       </c>
-      <c r="D34" s="68">
+      <c r="D34" s="67">
         <v>201</v>
       </c>
-      <c r="E34" s="69">
+      <c r="E34" s="68">
         <v>43766</v>
       </c>
-      <c r="F34" s="43">
+      <c r="F34" s="42">
         <v>43767</v>
       </c>
-      <c r="G34" s="36" t="s">
+      <c r="G34" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="H34" s="35" t="s">
+      <c r="H34" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="37">
+      <c r="B35" s="36">
         <v>10</v>
       </c>
-      <c r="C35" s="35">
+      <c r="C35" s="34">
         <v>6</v>
       </c>
-      <c r="D35" s="47">
+      <c r="D35" s="46">
         <v>201</v>
       </c>
-      <c r="E35" s="48">
+      <c r="E35" s="47">
         <v>43764</v>
       </c>
-      <c r="F35" s="43">
+      <c r="F35" s="42">
         <v>43765</v>
       </c>
-      <c r="G35" s="36" t="s">
+      <c r="G35" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="H35" s="35" t="s">
+      <c r="H35" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="57">
+      <c r="B36" s="56">
         <v>12</v>
       </c>
-      <c r="C36" s="42">
+      <c r="C36" s="41">
         <v>6</v>
       </c>
-      <c r="D36" s="77">
+      <c r="D36" s="76">
         <v>201</v>
       </c>
-      <c r="E36" s="78">
+      <c r="E36" s="77">
         <v>43765</v>
       </c>
-      <c r="F36" s="44">
+      <c r="F36" s="43">
         <v>43766</v>
       </c>
-      <c r="G36" s="66" t="s">
+      <c r="G36" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="H36" s="35" t="s">
+      <c r="H36" s="34" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="57"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="35"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="34"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="57"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="35"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="34"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="57"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="35"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="34"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="57"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="35"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="34"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="57"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="66"/>
-      <c r="H41" s="42"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>